<commit_message>
Se aareglo las formulas de la columna
</commit_message>
<xml_diff>
--- a/WinTestSearchGrid/ExcelEjemplo/DatosDeCarga.xlsx
+++ b/WinTestSearchGrid/ExcelEjemplo/DatosDeCarga.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/365c7072ff68b8fa/Documentos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\garfi\source\repos\WinTestSearchGrid\WinTestSearchGrid\ExcelEjemplo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{56905C86-5B4D-48A5-A6D4-25C717A12522}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{71299339-812A-46A1-92A7-0C4DB5D55AB7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A335A89F-81A9-4F4D-9D43-B8E8C128B91A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2A82CA9C-AF0E-4CBA-ABA5-D0F32F5284F3}"/>
   </bookViews>
@@ -450,15 +450,15 @@
         <v>Name1</v>
       </c>
       <c r="C2" t="str">
-        <f>$C$1 &amp; TEXT($A$2, "##")</f>
+        <f>$C$1 &amp; TEXT(A2, "##")</f>
         <v>Class1</v>
       </c>
       <c r="D2" t="str">
-        <f>$D$1 &amp; TEXT($A$2, "##")</f>
+        <f>$D$1 &amp; TEXT(A2, "##")</f>
         <v>Marks1</v>
       </c>
       <c r="E2" t="str">
-        <f>$E$1 &amp; TEXT($A$2, "##")</f>
+        <f>$E$1 &amp; TEXT(A2, "##")</f>
         <v>Gender1</v>
       </c>
     </row>
@@ -476,12 +476,12 @@
         <v>Class2</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" ref="D3:D17" si="2">$D$1 &amp; TEXT($A$2, "##")</f>
-        <v>Marks1</v>
+        <f t="shared" ref="D3:D17" si="2">$D$1 &amp; TEXT(A3, "##")</f>
+        <v>Marks2</v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" ref="E3:E17" si="3">$E$1 &amp; TEXT($A$2, "##")</f>
-        <v>Gender1</v>
+        <f t="shared" ref="E3:E17" si="3">$E$1 &amp; TEXT(A3, "##")</f>
+        <v>Gender2</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -499,11 +499,11 @@
       </c>
       <c r="D4" t="str">
         <f t="shared" si="2"/>
-        <v>Marks1</v>
+        <v>Marks3</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="3"/>
-        <v>Gender1</v>
+        <v>Gender3</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -521,11 +521,11 @@
       </c>
       <c r="D5" t="str">
         <f t="shared" si="2"/>
-        <v>Marks1</v>
+        <v>Marks4</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="3"/>
-        <v>Gender1</v>
+        <v>Gender4</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -543,11 +543,11 @@
       </c>
       <c r="D6" t="str">
         <f t="shared" si="2"/>
-        <v>Marks1</v>
+        <v>Marks5</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="3"/>
-        <v>Gender1</v>
+        <v>Gender5</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -565,11 +565,11 @@
       </c>
       <c r="D7" t="str">
         <f t="shared" si="2"/>
-        <v>Marks1</v>
+        <v>Marks6</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="3"/>
-        <v>Gender1</v>
+        <v>Gender6</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -587,11 +587,11 @@
       </c>
       <c r="D8" t="str">
         <f t="shared" si="2"/>
-        <v>Marks1</v>
+        <v>Marks7</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="3"/>
-        <v>Gender1</v>
+        <v>Gender7</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -609,11 +609,11 @@
       </c>
       <c r="D9" t="str">
         <f t="shared" si="2"/>
-        <v>Marks1</v>
+        <v>Marks8</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="3"/>
-        <v>Gender1</v>
+        <v>Gender8</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -631,11 +631,11 @@
       </c>
       <c r="D10" t="str">
         <f t="shared" si="2"/>
-        <v>Marks1</v>
+        <v>Marks9</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="3"/>
-        <v>Gender1</v>
+        <v>Gender9</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -653,11 +653,11 @@
       </c>
       <c r="D11" t="str">
         <f t="shared" si="2"/>
-        <v>Marks1</v>
+        <v>Marks10</v>
       </c>
       <c r="E11" t="str">
         <f t="shared" si="3"/>
-        <v>Gender1</v>
+        <v>Gender10</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -675,11 +675,11 @@
       </c>
       <c r="D12" t="str">
         <f t="shared" si="2"/>
-        <v>Marks1</v>
+        <v>Marks11</v>
       </c>
       <c r="E12" t="str">
         <f t="shared" si="3"/>
-        <v>Gender1</v>
+        <v>Gender11</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -697,11 +697,11 @@
       </c>
       <c r="D13" t="str">
         <f t="shared" si="2"/>
-        <v>Marks1</v>
+        <v>Marks12</v>
       </c>
       <c r="E13" t="str">
         <f t="shared" si="3"/>
-        <v>Gender1</v>
+        <v>Gender12</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -719,11 +719,11 @@
       </c>
       <c r="D14" t="str">
         <f t="shared" si="2"/>
-        <v>Marks1</v>
+        <v>Marks13</v>
       </c>
       <c r="E14" t="str">
         <f t="shared" si="3"/>
-        <v>Gender1</v>
+        <v>Gender13</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -741,11 +741,11 @@
       </c>
       <c r="D15" t="str">
         <f t="shared" si="2"/>
-        <v>Marks1</v>
+        <v>Marks14</v>
       </c>
       <c r="E15" t="str">
         <f t="shared" si="3"/>
-        <v>Gender1</v>
+        <v>Gender14</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -763,11 +763,11 @@
       </c>
       <c r="D16" t="str">
         <f t="shared" si="2"/>
-        <v>Marks1</v>
+        <v>Marks15</v>
       </c>
       <c r="E16" t="str">
         <f t="shared" si="3"/>
-        <v>Gender1</v>
+        <v>Gender15</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -785,11 +785,11 @@
       </c>
       <c r="D17" t="str">
         <f t="shared" si="2"/>
-        <v>Marks1</v>
+        <v>Marks16</v>
       </c>
       <c r="E17" t="str">
         <f t="shared" si="3"/>
-        <v>Gender1</v>
+        <v>Gender16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>